<commit_message>
add code and files
</commit_message>
<xml_diff>
--- a/plots/source-data.xlsx
+++ b/plots/source-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neil/GitHubRepo/Projects/PreySelection/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B8469D-6432-D340-9EF2-3031996C0215}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972C44AD-ADB4-2047-BB7F-DB29D6050133}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="23300" windowWidth="22740" windowHeight="15400" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10420" yWindow="720" windowWidth="18080" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 2a" sheetId="2" r:id="rId1"/>
@@ -23,14 +23,23 @@
     <sheet name="Figure 3d" sheetId="7" r:id="rId8"/>
     <sheet name="Figure 4a" sheetId="8" r:id="rId9"/>
     <sheet name="Figure 4b" sheetId="11" r:id="rId10"/>
-    <sheet name="Table 1" sheetId="12" r:id="rId11"/>
+    <sheet name="SuppFigure1a" sheetId="17" r:id="rId11"/>
+    <sheet name="SuppFigure1b" sheetId="18" r:id="rId12"/>
+    <sheet name="SuppFigure1c" sheetId="19" r:id="rId13"/>
+    <sheet name="SuppFigure1d" sheetId="20" r:id="rId14"/>
+    <sheet name="SuppFigure2" sheetId="21" r:id="rId15"/>
+    <sheet name="SuppFigure3" sheetId="15" r:id="rId16"/>
+    <sheet name="SuppFigure4a" sheetId="13" r:id="rId17"/>
+    <sheet name="SuppFigure4b" sheetId="14" r:id="rId18"/>
+    <sheet name="Table 1" sheetId="12" r:id="rId19"/>
+    <sheet name="SuppTable 1" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="116">
   <si>
     <t>Figure 2a</t>
   </si>
@@ -290,15 +299,195 @@
   <si>
     <t>0.123 [95% CI = 0.0528, 0.2403]</t>
   </si>
+  <si>
+    <t>Supp 4a</t>
+  </si>
+  <si>
+    <t>simulations: Perseverance Model</t>
+  </si>
+  <si>
+    <t>Supp 4b</t>
+  </si>
+  <si>
+    <t>Supp 3</t>
+  </si>
+  <si>
+    <t>Supp 1a</t>
+  </si>
+  <si>
+    <t>Supp 1b</t>
+  </si>
+  <si>
+    <t>Supp 1c</t>
+  </si>
+  <si>
+    <t>Supp 1d</t>
+  </si>
+  <si>
+    <t>HRLD</t>
+  </si>
+  <si>
+    <t>LRLD</t>
+  </si>
+  <si>
+    <t>LRHD</t>
+  </si>
+  <si>
+    <t>93.93 (3.33)</t>
+  </si>
+  <si>
+    <t>λ</t>
+  </si>
+  <si>
+    <t>Symmetric Learn Options Model</t>
+  </si>
+  <si>
+    <t>Asymmetric Learn Options Model</t>
+  </si>
+  <si>
+    <t>67.94 (4.04)</t>
+  </si>
+  <si>
+    <t>62.28 (2.68)</t>
+  </si>
+  <si>
+    <t>47.92 (2.82)</t>
+  </si>
+  <si>
+    <t>77.67 (3.53)</t>
+  </si>
+  <si>
+    <t>65.79 (3.39)</t>
+  </si>
+  <si>
+    <t>0.4072
+95% CI = [0.2789, 0.5463]
+(3.39)</t>
+  </si>
+  <si>
+    <t>0.5489
+95% CI = [0.3864, 0.7035]</t>
+  </si>
+  <si>
+    <t>0.2390
+95% CI = [0.1762, 0.3123]</t>
+  </si>
+  <si>
+    <t>0.3076
+95% CI = [0.2213, 0.4062]</t>
+  </si>
+  <si>
+    <t>0.3332
+95% CI = 
+[0.2149, 0.4710]</t>
+  </si>
+  <si>
+    <t>0.3285
+95% CI = 
+[0.2057, 0.4733]</t>
+  </si>
+  <si>
+    <t>0.0177
+95% CI = [0.005, 0.0515]</t>
+  </si>
+  <si>
+    <t>0.0066
+95% CI = [0.0035, 0.0118]</t>
+  </si>
+  <si>
+    <t>0.0213
+95% CI = [0.007, 0.056]</t>
+  </si>
+  <si>
+    <t>0.0051
+95% CI = [0.0031, 0.0082]</t>
+  </si>
+  <si>
+    <t>0.1116
+95% CI = 
+[0.0491, 0.2171]</t>
+  </si>
+  <si>
+    <t>0.0293
+95% CI = 
+[0.0218, 0.0389]</t>
+  </si>
+  <si>
+    <t>0.0020
+95% CI = [0.0011, 0.0037]</t>
+  </si>
+  <si>
+    <t>0.86
+95% CI = [0.59, 1.13]</t>
+  </si>
+  <si>
+    <t>-1.82
+95% CI = 
+[-2.54, -1.11]</t>
+  </si>
+  <si>
+    <t>0.09
+95% CI = [0.08, 0.10]</t>
+  </si>
+  <si>
+    <t>0.09
+95% CI = [0.08,0.11]</t>
+  </si>
+  <si>
+    <t>0.69
+95% CI = [0.40, 0.98]</t>
+  </si>
+  <si>
+    <t>0.10
+95% CI = [0.09, 0.12]</t>
+  </si>
+  <si>
+    <t>0.11
+95% CI = 
+[-2.00, -0.74]</t>
+  </si>
+  <si>
+    <t>-1.37
+95% CI = 
+[-2.00, -0.74]</t>
+  </si>
+  <si>
+    <t>0.0022
+95% CI = [0.0014, 0.0034]</t>
+  </si>
+  <si>
+    <t>0.0179
+95% CI = 
+[0.0139, 0.0227]</t>
+  </si>
+  <si>
+    <t>0.11
+95% CI = 
+[0.09, 0.13]</t>
+  </si>
+  <si>
+    <t>-1.01
+95% CI = 
+[-1.44, -0.57]</t>
+  </si>
+  <si>
+    <t>0.65
+95% CI = 
+[0.38, 0.93]</t>
+  </si>
+  <si>
+    <t>Supp Table 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,7 +569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -404,28 +593,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -441,13 +608,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -457,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -481,44 +648,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,36 +1039,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="C4" s="9" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>3</v>
@@ -909,7 +1089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -933,7 +1113,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -957,7 +1137,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -967,7 +1147,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -976,7 +1156,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -985,7 +1165,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1006,27 +1186,27 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1035,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1046,7 +1226,7 @@
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1057,22 +1237,22 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1084,320 +1264,1380 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A7C6A9-6A7D-FD46-8A4D-B7ED5D5F7D8F}">
+  <dimension ref="A3:J11"/>
+  <sheetViews>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.98973686000000005</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.96972773000000001</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.50573822000000002</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.73939041999999999</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.37957194999999999</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.47320076999999999</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.12345737</v>
+      </c>
+      <c r="J6" s="21">
+        <v>1.882122E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>3.5983899999999999E-3</v>
+      </c>
+      <c r="D7" s="18">
+        <v>9.8678770000000006E-3</v>
+      </c>
+      <c r="E7" s="18">
+        <v>8.1859824999999997E-2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>7.6407632000000003E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>8.9219186000000006E-2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>8.9819271000000006E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>3.5959704000000002E-2</v>
+      </c>
+      <c r="J7" s="21">
+        <v>4.5505950000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734A1F7B-E724-6946-823D-D87763C9C50F}">
+  <dimension ref="A3:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.99660000000000004</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.95960000000000001</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.66349999999999998</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.82889999999999997</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.18820000000000001</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.77239999999999998</v>
+      </c>
+      <c r="I6" s="18">
+        <v>5.3499999999999999E-2</v>
+      </c>
+      <c r="J6" s="18">
+        <v>4.3200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>8.14E-2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>5.2600000000000001E-2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>5.3100000000000001E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD22EB9-980E-F143-AC06-3BAFC1F7E9F7}">
+  <dimension ref="A3:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.98369121999999998</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.98253354000000004</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.42683879000000002</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.64956130000000001</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.35947642000000002</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.55996420000000002</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.21935878</v>
+      </c>
+      <c r="J6" s="21">
+        <v>2.2525010000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>7.1606760000000004E-3</v>
+      </c>
+      <c r="D7" s="21">
+        <v>8.1689339999999992E-3</v>
+      </c>
+      <c r="E7" s="18">
+        <v>8.5667038000000001E-2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>9.5944495000000005E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>7.0605917000000004E-2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>8.3381227000000002E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>4.3723024999999999E-2</v>
+      </c>
+      <c r="J7" s="21">
+        <v>7.3684839999999998E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F64F9C-BDD0-6947-B466-315B7A0EC613}">
+  <dimension ref="A3:J11"/>
+  <sheetViews>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="D6" sqref="C6:J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.99060000000000004</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.9738</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.62090000000000001</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.82279999999999998</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.3125</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.83789999999999998</v>
+      </c>
+      <c r="I6" s="18">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="J6" s="18">
+        <v>8.7800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>3.6862650000000002E-3</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1.1184563999999999E-2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>9.4204450999999995E-2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>6.2479538000000001E-2</v>
+      </c>
+      <c r="G7" s="18">
+        <v>7.7587054000000003E-2</v>
+      </c>
+      <c r="H7" s="18">
+        <v>5.2014790999999998E-2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>3.9159368E-2</v>
+      </c>
+      <c r="J7" s="21">
+        <v>2.4386152000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22BA63A-C293-9C47-ABD1-5EB0333B5C36}">
+  <dimension ref="A2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="C4" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>13.45011</v>
+      </c>
+      <c r="D6" s="18">
+        <v>13.446529999999999</v>
+      </c>
+      <c r="E6" s="21">
+        <v>17.378209999999999</v>
+      </c>
+      <c r="F6" s="18">
+        <v>10.434150000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1.130512</v>
+      </c>
+      <c r="D7" s="18">
+        <v>1.6196809999999999</v>
+      </c>
+      <c r="E7" s="18">
+        <v>2.126144</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1.032489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889098CC-A3EC-5249-9A7C-0CA504D98149}">
+  <dimension ref="A2:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.50119999999999998</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="E7" s="18">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5117FA5E-30F0-314D-92BD-007BB1BFFEE1}">
+  <dimension ref="A2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="C4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.1142</v>
+      </c>
+      <c r="F6">
+        <v>0.11609999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="17">
+        <v>7.5308999999999999E-4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>7.6501E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F469FC-957C-A14A-BB32-FE8583F9C1C3}">
+  <dimension ref="A2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="6" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="C4" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.1129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="17">
+        <v>7.7895999999999998E-4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>7.6239000000000005E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81ABBDE8-1207-3C4E-A6C8-A34A902A60AA}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19:H21"/>
+    <sheetView zoomScale="93" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="10"/>
-    <col min="2" max="2" width="30.1640625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="10.83203125" style="9"/>
+    <col min="2" max="2" width="30.1640625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1"/>
-    <row r="2" spans="1:8" ht="20" thickBot="1">
-      <c r="D2" s="21" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" ht="15">
-      <c r="B4" s="18" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.15">
+      <c r="B4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" ht="14" customHeight="1">
-      <c r="B5" s="20" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="B6" s="20"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" s="20"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" s="20" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B8" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="26" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="20"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="B10" s="20"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="1:8" ht="15">
-      <c r="B11" s="18" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.15">
+      <c r="B11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" s="20" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="23" t="s">
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="26" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="B13" s="20"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" s="20"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="20" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="23" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="20"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="20"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-    </row>
-    <row r="18" spans="2:8" ht="15">
-      <c r="B18" s="18" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.15">
+      <c r="B18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="20" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="23" t="s">
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="23" t="s">
+      <c r="H19" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="20"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="20"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="20" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="23" t="s">
+      <c r="D22" s="25"/>
+      <c r="E22" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="20"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="20"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="42">
@@ -1407,13 +2647,8 @@
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="G12:G14"/>
     <mergeCell ref="H12:H14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D19:D21"/>
     <mergeCell ref="G19:G21"/>
     <mergeCell ref="H19:H21"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="D15:D17"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="F19:F21"/>
@@ -1421,6 +2656,7 @@
     <mergeCell ref="F15:F17"/>
     <mergeCell ref="E22:E24"/>
     <mergeCell ref="F22:F24"/>
+    <mergeCell ref="D19:D21"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
@@ -1431,8 +2667,10 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="H8:H10"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="D15:D17"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="B12:B14"/>
@@ -1443,6 +2681,8 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1456,32 +2696,32 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="C4" s="9" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>3</v>
@@ -1502,7 +2742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1526,7 +2766,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1550,7 +2790,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1560,7 +2800,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1569,7 +2809,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1578,7 +2818,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1586,6 +2826,414 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC125ED-9CFA-644A-AC2F-9AE71C125FAE}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1640625" style="9" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="B4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B7" s="23"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B8" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="B11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B12" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B15" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H15" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.15">
+      <c r="B18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B22" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="48">
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1599,29 +3247,29 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -1633,7 +3281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1648,7 +3296,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1663,26 +3311,26 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1698,32 +3346,32 @@
   <dimension ref="A2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -1735,7 +3383,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1750,7 +3398,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1765,26 +3413,26 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1800,38 +3448,38 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1852,7 +3500,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1862,8 +3510,20 @@
       <c r="D6" s="8">
         <v>0.17599999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="E6">
+        <v>0.11310000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.1085</v>
+      </c>
+      <c r="G6">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.1817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1873,23 +3533,39 @@
       <c r="D7" s="8">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="E7" s="17">
+        <v>7.5975999999999995E-4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>7.5834000000000003E-4</v>
+      </c>
+      <c r="G7" s="17">
+        <v>8.1055000000000005E-4</v>
+      </c>
+      <c r="H7" s="17">
+        <v>7.3698000000000004E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1907,38 +3583,38 @@
   <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A9" sqref="A9:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1959,7 +3635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -1969,8 +3645,20 @@
       <c r="D6" s="8">
         <v>0.17899999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="E6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.1154</v>
+      </c>
+      <c r="G6">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H6">
+        <v>0.18410000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1980,23 +3668,39 @@
       <c r="D7" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="E7" s="17">
+        <v>7.6446999999999995E-4</v>
+      </c>
+      <c r="F7" s="17">
+        <v>7.8536999999999997E-4</v>
+      </c>
+      <c r="G7" s="17">
+        <v>7.5927999999999998E-4</v>
+      </c>
+      <c r="H7" s="17">
+        <v>6.9079999999999999E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -2017,28 +3721,28 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>13</v>
@@ -2047,7 +3751,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -2059,7 +3763,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2071,23 +3775,23 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -2106,28 +3810,28 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>13</v>
@@ -2136,7 +3840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -2148,7 +3852,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2160,23 +3864,23 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -2195,32 +3899,32 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
         <v>17</v>
@@ -2235,7 +3939,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
@@ -2252,7 +3956,7 @@
         <v>10.273</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
@@ -2269,23 +3973,23 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
     </row>
   </sheetData>

</xml_diff>